<commit_message>
hyperparameter tuning in boosting and paramter exploration in logistic regression
</commit_message>
<xml_diff>
--- a/Model Evaluation.xlsx
+++ b/Model Evaluation.xlsx
@@ -11,7 +11,34 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
+  <si>
+    <t>Logistic Regression</t>
+  </si>
+  <si>
+    <t>multi_class</t>
+  </si>
+  <si>
+    <t>solver</t>
+  </si>
+  <si>
+    <t>micro-avg</t>
+  </si>
+  <si>
+    <t>macro-avg</t>
+  </si>
+  <si>
+    <t>weighted avg</t>
+  </si>
+  <si>
+    <t>ovr</t>
+  </si>
+  <si>
+    <t>newton-cg</t>
+  </si>
+  <si>
+    <t>multinomial</t>
+  </si>
   <si>
     <t>Model</t>
   </si>
@@ -20,12 +47,6 @@
   </si>
   <si>
     <t>macro avg</t>
-  </si>
-  <si>
-    <t>weighted avg</t>
-  </si>
-  <si>
-    <t>Logistic Regression</t>
   </si>
   <si>
     <t>Logistic Regression After 
@@ -35,13 +56,31 @@
   <si>
     <t>Logistic Regression After 
 SMOTE Oversampling</t>
+  </si>
+  <si>
+    <t>learning_rate</t>
+  </si>
+  <si>
+    <t>max_depth</t>
+  </si>
+  <si>
+    <t>n_estimators</t>
+  </si>
+  <si>
+    <t>subsample</t>
+  </si>
+  <si>
+    <t>weighted-avg</t>
+  </si>
+  <si>
+    <t>xgbclassifier</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -51,15 +90,36 @@
     <font>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="Monospace"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FFFF"/>
+        <bgColor rgb="FF00FFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -68,11 +128,29 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -291,63 +369,202 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="32.38"/>
+    <col customWidth="1" min="1" max="1" width="22.38"/>
+    <col customWidth="1" min="2" max="2" width="20.13"/>
   </cols>
   <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
     <row r="3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0.64</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0.48</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0.66</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.53</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="B7" s="6">
+        <v>0.64</v>
+      </c>
+      <c r="C7" s="6">
+        <v>0.45</v>
+      </c>
+      <c r="D7" s="6">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="6">
+        <v>0.66</v>
+      </c>
+      <c r="C8" s="6">
+        <v>0.53</v>
+      </c>
+      <c r="D8" s="6">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="6">
+        <v>0.54</v>
+      </c>
+      <c r="C9" s="6">
+        <v>0.47</v>
+      </c>
+      <c r="D9" s="6">
+        <v>0.57</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="s">
+      <c r="G11" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1">
+      <c r="H11" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="7">
+        <v>0.0824936125406674</v>
+      </c>
+      <c r="C12" s="6">
+        <v>16.0</v>
+      </c>
+      <c r="D12" s="6">
+        <v>113.0</v>
+      </c>
+      <c r="E12" s="7">
+        <v>0.539472383193716</v>
+      </c>
+      <c r="F12" s="6">
+        <v>0.66</v>
+      </c>
+      <c r="G12" s="6">
+        <v>0.52</v>
+      </c>
+      <c r="H12" s="6">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="7">
+        <v>0.0903022531263533</v>
+      </c>
+      <c r="C13" s="6">
+        <v>19.0</v>
+      </c>
+      <c r="D13" s="6">
+        <v>127.0</v>
+      </c>
+      <c r="E13" s="6">
+        <v>0.652017589584536</v>
+      </c>
+      <c r="F13" s="6">
         <v>0.64</v>
       </c>
-      <c r="C4" s="1">
-        <v>0.45</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0.62</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="1">
-        <v>0.66</v>
-      </c>
-      <c r="C5" s="1">
-        <v>0.53</v>
-      </c>
-      <c r="D5" s="1">
+      <c r="G13" s="6">
+        <v>0.49</v>
+      </c>
+      <c r="H13" s="6">
         <v>0.65</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="1">
-        <v>0.54</v>
-      </c>
-      <c r="C6" s="1">
-        <v>0.47</v>
-      </c>
-      <c r="D6" s="1">
-        <v>0.57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>